<commit_message>
tuki excel-importille henkilö-oidilla. toimii myös jos useammalla henkilöllä sama synt.aika
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_oidilla.xlsx
+++ b/src/test/resources/erillishaku_oidilla.xlsx
@@ -50,10 +50,10 @@
     <t>Tuomas</t>
   </si>
   <si>
-    <t>010101-123N</t>
-  </si>
-  <si>
-    <t>1.1.1901</t>
+    <t>1.1.1980</t>
+  </si>
+  <si>
+    <t>hakija1</t>
   </si>
   <si>
     <t>HYVAKSYTTY</t>
@@ -69,8 +69,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -145,9 +146,10 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -169,12 +171,12 @@
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
+      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="D3"/>
       <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="1">
@@ -213,13 +215,13 @@
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Test with KK haku
fix test data to include also new fields
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_oidilla.xlsx
+++ b/src/test/resources/erillishaku_oidilla.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve">Sukunimi</t>
   </si>
@@ -64,6 +64,33 @@
     <t xml:space="preserve">Julkaistavissa</t>
   </si>
   <si>
+    <t xml:space="preserve">Asiointikieli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puhelinnumero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osoite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postinumero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postitoimipaikka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asuinmaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kansalaisuus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kotikunta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pohjakoulutus maa (toinen aste)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hakkarainen</t>
   </si>
   <si>
@@ -98,16 +125,32 @@
   </si>
   <si>
     <t xml:space="preserve">JULKAISTAVISSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">045123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testitie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helsinki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -200,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,15 +260,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,19 +293,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="10.0074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8037037037037"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="1" width="10.0074074074074"/>
-    <col collapsed="false" hidden="false" max="258" min="15" style="1" width="7.44074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="259" style="0" width="7.44074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="10.6888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6555555555556"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="1" width="10.6888888888889"/>
+    <col collapsed="false" hidden="false" max="260" min="15" style="1" width="7.95185185185185"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -304,176 +350,302 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="K2" s="6" t="n">
         <v>42538</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add toisen asteen suoritus column
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_oidilla.xlsx
+++ b/src/test/resources/erillishaku_oidilla.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t xml:space="preserve">Sukunimi</t>
   </si>
@@ -88,6 +88,9 @@
     <t xml:space="preserve">Kotikunta</t>
   </si>
   <si>
+    <t xml:space="preserve">Toisen asteen pohjakoulutus suoritettu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pohjakoulutus maa (toinen aste)</t>
   </si>
   <si>
@@ -140,6 +143,9 @@
   </si>
   <si>
     <t xml:space="preserve">FIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyllä</t>
   </si>
 </sst>
 </file>
@@ -293,18 +299,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
+      <selection pane="topLeft" activeCell="W2" activeCellId="0" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="10.6888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6555555555556"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="1" width="10.6888888888889"/>
-    <col collapsed="false" hidden="false" max="260" min="15" style="1" width="7.95185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="11.4592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5962962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="1" width="11.4592592592593"/>
+    <col collapsed="false" hidden="false" max="261" min="15" style="1" width="8.46666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="262" style="0" width="8.98148148148148"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -377,74 +384,80 @@
       <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K2" s="6" t="n">
         <v>42538</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>39</v>
+      <c r="W2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -471,6 +484,7 @@
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
@@ -496,6 +510,7 @@
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
@@ -521,6 +536,7 @@
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
@@ -546,6 +562,7 @@
       <c r="U6" s="7"/>
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
@@ -571,6 +588,7 @@
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
@@ -596,6 +614,7 @@
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
@@ -621,6 +640,7 @@
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
@@ -646,6 +666,7 @@
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Korjaa testit excelin tuonnille.
Testi-exceleihin lisätty kenttä 'Lukuvuosimaksuvelvollisuus'.
Lisäksi lisätty hakutyyppiin perustuva tarkistus excelin vientiin.
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_oidilla.xlsx
+++ b/src/test/resources/erillishaku_oidilla.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t xml:space="preserve">Sukunimi</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Ilmoittautumistila</t>
   </si>
   <si>
+    <t xml:space="preserve">Lukuvuosimaksuvelvollisuus</t>
+  </si>
+  <si>
     <t xml:space="preserve">Julkaistavissa</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">EI_TEHTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EI</t>
   </si>
   <si>
     <t xml:space="preserve">JULKAISTAVISSA</t>
@@ -299,19 +305,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W2" activeCellId="0" sqref="W2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5962962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="1" width="11.4592592592593"/>
-    <col collapsed="false" hidden="false" max="261" min="15" style="1" width="8.46666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="262" style="0" width="8.98148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="12.3407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.6740740740741"/>
+    <col collapsed="false" hidden="false" max="15" min="5" style="1" width="12.3407407407407"/>
+    <col collapsed="false" hidden="false" max="262" min="16" style="1" width="9.14444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="263" style="0" width="9.75185185185185"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -360,10 +366,10 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
@@ -387,77 +393,83 @@
       <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K2" s="6" t="n">
         <v>42538</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="P2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="R2" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="S2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="T2" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="U2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>40</v>
+      <c r="X2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -485,6 +497,7 @@
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
@@ -511,6 +524,7 @@
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
@@ -537,6 +551,7 @@
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
@@ -563,6 +578,7 @@
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
@@ -589,6 +605,7 @@
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
@@ -615,6 +632,7 @@
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
@@ -641,6 +659,7 @@
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
@@ -667,6 +686,7 @@
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -674,7 +694,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;L&amp;"Arial,Regular"	&amp;P</oddFooter>

</xml_diff>

<commit_message>
Päivitetty yksikkötestit vastaamaan muutoksia
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_oidilla.xlsx
+++ b/src/test/resources/erillishaku_oidilla.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terip1/IdeaProjects/Opetushallitus/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="46600" windowHeight="16540"/>
+    <workbookView xWindow="33000" yWindow="3480" windowWidth="28800" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -124,9 +132,6 @@
     </r>
   </si>
   <si>
-    <t>1.1.1980</t>
-  </si>
-  <si>
     <t>MIES</t>
   </si>
   <si>
@@ -173,6 +178,9 @@
   </si>
   <si>
     <t>Maksun tila</t>
+  </si>
+  <si>
+    <t>01.01.1980</t>
   </si>
 </sst>
 </file>
@@ -331,6 +339,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1409,21 +1422,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW10"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="9" width="8.625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
-    <col min="12" max="257" width="8.625" style="1" customWidth="1"/>
+    <col min="12" max="30" width="8.625" style="1" customWidth="1"/>
+    <col min="31" max="257" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17" customHeight="1">
+    <row r="1" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1479,7 +1493,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>18</v>
@@ -1515,7 +1529,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="17" customHeight="1">
+    <row r="2" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1527,22 +1541,22 @@
         <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="6"/>
@@ -1552,50 +1566,50 @@
         <v>42538</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="3" spans="1:30" ht="19" customHeight="1">
+    <row r="3" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1627,7 +1641,7 @@
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
     </row>
-    <row r="4" spans="1:30" ht="19" customHeight="1">
+    <row r="4" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1659,7 +1673,7 @@
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
     </row>
-    <row r="5" spans="1:30" ht="19" customHeight="1">
+    <row r="5" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1691,7 +1705,7 @@
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
     </row>
-    <row r="6" spans="1:30" ht="19" customHeight="1">
+    <row r="6" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1723,7 +1737,7 @@
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
     </row>
-    <row r="7" spans="1:30" ht="19" customHeight="1">
+    <row r="7" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1755,7 +1769,7 @@
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
     </row>
-    <row r="8" spans="1:30" ht="19" customHeight="1">
+    <row r="8" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1787,7 +1801,7 @@
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
     </row>
-    <row r="9" spans="1:30" ht="19" customHeight="1">
+    <row r="9" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1819,7 +1833,7 @@
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
     </row>
-    <row r="10" spans="1:30" ht="19" customHeight="1">
+    <row r="10" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1860,10 +1874,5 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Arial,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OY-3070 validate presence of hakemus OID when henkilo OID present
</commit_message>
<xml_diff>
--- a/src/test/resources/erillishaku_oidilla.xlsx
+++ b/src/test/resources/erillishaku_oidilla.xlsx
@@ -1,33 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terip1/IdeaProjects/Opetushallitus/valintaperusteet/valintalaskentakoostepalvelu/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="33000" yWindow="3480" windowWidth="28800" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>Sukunimi</t>
   </si>
@@ -83,6 +67,9 @@
     <t>Lukuvuosimaksuvelvollisuus</t>
   </si>
   <si>
+    <t>Maksun tila</t>
+  </si>
+  <si>
     <t>Julkaistavissa</t>
   </si>
   <si>
@@ -114,6 +101,24 @@
   </si>
   <si>
     <t>Pohjakoulutus maa (toinen aste)</t>
+  </si>
+  <si>
+    <t>Kutsumanimi</t>
+  </si>
+  <si>
+    <t>Syntymäpaikka</t>
+  </si>
+  <si>
+    <t>Passin numero</t>
+  </si>
+  <si>
+    <t>Kansallinen ID-tunnus</t>
+  </si>
+  <si>
+    <t>Kaupunki ja maa</t>
+  </si>
+  <si>
+    <t>Hakemus-oid</t>
   </si>
   <si>
     <t>Hakkarainen</t>
@@ -132,10 +137,13 @@
     </r>
   </si>
   <si>
+    <t>01.01.1980</t>
+  </si>
+  <si>
     <t>MIES</t>
   </si>
   <si>
-    <t>hakija1</t>
+    <t>Hakijaoid1</t>
   </si>
   <si>
     <t>FI</t>
@@ -177,21 +185,31 @@
     <t>Kyllä</t>
   </si>
   <si>
-    <t>Maksun tila</t>
-  </si>
-  <si>
-    <t>01.01.1980</t>
+    <t>Hakemus1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -248,107 +266,61 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="001FB714"/>
-      <rgbColor rgb="000000D4"/>
-      <rgbColor rgb="00FCF305"/>
-      <rgbColor rgb="00F20884"/>
-      <rgbColor rgb="0000ABEA"/>
-      <rgbColor rgb="00900000"/>
-      <rgbColor rgb="00006411"/>
-      <rgbColor rgb="00000090"/>
-      <rgbColor rgb="0090713A"/>
-      <rgbColor rgb="004600A5"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -390,14 +362,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -540,17 +512,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -569,19 +541,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -599,7 +571,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -625,7 +597,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -651,7 +623,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -677,7 +649,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -703,7 +675,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -729,7 +701,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -755,7 +727,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -781,7 +753,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -807,7 +779,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -820,32 +792,26 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -864,7 +830,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -890,7 +856,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -916,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -942,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -968,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -994,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1020,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1046,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1072,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1098,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1111,15 +1077,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1133,7 +1093,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1152,19 +1112,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1182,7 +1142,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1208,7 +1168,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1234,7 +1194,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1260,7 +1220,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1286,7 +1246,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1312,7 +1272,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1338,7 +1298,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1364,7 +1324,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1390,7 +1350,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1403,160 +1363,169 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD10"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="9" width="8.625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.625" style="1" customWidth="1"/>
-    <col min="12" max="30" width="8.625" style="1" customWidth="1"/>
-    <col min="31" max="257" width="8.625" customWidth="1"/>
+    <col min="12" max="36" width="8.625" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="17" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="S1" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="T1" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="U1" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="V1" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="W1" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="X1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Y1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="Z1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AA1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AB1" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AC1" t="s" s="2">
         <v>28</v>
       </c>
+      <c r="AD1" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s" s="2">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
+    <row r="2" ht="17" customHeight="1">
+      <c r="A2" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>37</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>36</v>
+      <c r="D2" t="s" s="4">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s" s="2">
+        <v>44</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="6"/>
@@ -1565,51 +1534,61 @@
       <c r="O2" s="6">
         <v>42538</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Q2" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="U2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="W2" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="X2" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="Y2" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="Z2" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AA2" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AB2" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AC2" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="AD2" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="AE2" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>45</v>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" t="s" s="2">
+        <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="19" customHeight="1">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1640,8 +1619,14 @@
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" ht="19" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1672,8 +1657,14 @@
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="19" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1704,8 +1695,14 @@
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" ht="19" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1736,8 +1733,14 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" ht="19" customHeight="1">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1768,8 +1771,14 @@
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" ht="19" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1800,8 +1809,14 @@
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
     </row>
-    <row r="9" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" ht="19" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1832,8 +1847,14 @@
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
     </row>
-    <row r="10" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" ht="19" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1864,13 +1885,19 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="tuomas.hakkarainen@example.com"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180599999999998" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Arial,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>